<commit_message>
Plan de Sprint modificado
</commit_message>
<xml_diff>
--- a/Storys/Storys/Hoja1 (version 1).xlsx
+++ b/Storys/Storys/Hoja1 (version 1).xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="99">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -269,7 +269,13 @@
     <t xml:space="preserve">Sprint 3 (16/11/18 - 30/11/18)</t>
   </si>
   <si>
-    <t xml:space="preserve">Sprint 4 (30/11/18 - 13/12/18)</t>
+    <t xml:space="preserve">Sprint 4 (27/11/18 – 28/11/18)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 5 (29/11/18 – 5/12/18)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 6 (6/12/18 – 12/12/18)</t>
   </si>
   <si>
     <t xml:space="preserve">Login Ver. 1</t>
@@ -278,21 +284,18 @@
     <t xml:space="preserve">Alta Usuario Ver. 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Estudios Particular (Encuestador)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Estudios Particular (Analista)</t>
   </si>
   <si>
-    <t xml:space="preserve">Estudios Particular (Encuestador)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total </t>
   </si>
   <si>
     <t xml:space="preserve">Login Ver. 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Edgar</t>
-  </si>
-  <si>
     <t xml:space="preserve">Marisol</t>
   </si>
   <si>
@@ -315,9 +318,6 @@
   </si>
   <si>
     <t xml:space="preserve">edgar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Emmanuel</t>
   </si>
 </sst>
 </file>
@@ -327,12 +327,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -350,84 +351,14 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
     </font>
@@ -435,9 +366,10 @@
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -446,62 +378,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFE2EFD9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFF7CAAC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFD9E2F3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFB4C6E7"/>
-        <bgColor rgb="FFC5E0B3"/>
+        <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD9E2F3"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFE2EFD9"/>
       </patternFill>
     </fill>
     <fill>
@@ -513,7 +403,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCDFF"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFD9E2F3"/>
       </patternFill>
     </fill>
     <fill>
@@ -537,7 +427,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF7CAAC"/>
-        <bgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFFFAFAF"/>
       </patternFill>
     </fill>
     <fill>
@@ -549,31 +439,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC5E0B3"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFE2EFD9"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -584,7 +459,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -608,59 +483,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -669,67 +493,67 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="16" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="15" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="18" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="19" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="18" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="19" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -737,50 +561,37 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFFCDFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB4C6E7"/>
@@ -788,9 +599,9 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFE2EFD9"/>
+      <rgbColor rgb="FFC5E0B3"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFD9E2F3"/>
       <rgbColor rgb="FF000080"/>
@@ -802,12 +613,12 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00B0F0"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFE2EFD9"/>
       <rgbColor rgb="FFFFE598"/>
-      <rgbColor rgb="FFC5E0B3"/>
+      <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFFAFAF"/>
-      <rgbColor rgb="FFFFCDFF"/>
+      <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF7CAAC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
@@ -2715,27 +2526,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:K35"/>
+  <dimension ref="B1:M35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I21" activeCellId="0" sqref="I21"/>
+      <selection pane="topLeft" activeCell="L27" activeCellId="0" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="2.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="32.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="22.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="13" style="0" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="32.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="3.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="14" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="27" style="0" width="14.43"/>
   </cols>
   <sheetData>
@@ -2750,53 +2562,83 @@
       <c r="F2" s="18" t="s">
         <v>81</v>
       </c>
+      <c r="H2" s="0" t="s">
+        <v>82</v>
+      </c>
       <c r="J2" s="18" t="s">
-        <v>82</v>
+        <v>83</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="G3" s="19" t="n">
+      <c r="D3" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G3" s="20" t="n">
         <v>2</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="19" t="n">
+      <c r="I3" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="20" t="n">
+        <v>13</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="19" t="n">
+      <c r="M3" s="20" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="G4" s="19" t="n">
+      <c r="D4" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G4" s="20" t="n">
         <v>1</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I4" s="19" t="n">
+      <c r="I4" s="20" t="n">
         <v>2</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="K4" s="20" t="n">
+        <v>13</v>
+      </c>
+      <c r="L4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K4" s="19" t="n">
+      <c r="M4" s="20" t="n">
         <v>13</v>
       </c>
     </row>
@@ -2807,19 +2649,19 @@
       <c r="C5" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="G5" s="19" t="n">
+      <c r="G5" s="20" t="n">
         <v>3</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="I5" s="19" t="n">
+        <v>88</v>
+      </c>
+      <c r="I5" s="20" t="n">
         <v>5</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="L5" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="K5" s="19" t="n">
+      <c r="M5" s="20" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2830,26 +2672,14 @@
       <c r="C6" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="G6" s="19" t="n">
+      <c r="G6" s="20" t="n">
         <v>3</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="19" t="n">
+      <c r="I6" s="20" t="n">
         <v>8</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="K6" s="19" t="n">
-        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2859,51 +2689,39 @@
       <c r="C7" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G7" s="19" t="n">
+      <c r="G7" s="20" t="n">
         <v>3</v>
       </c>
       <c r="H7" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="19" t="n">
+      <c r="I7" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="J7" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="K7" s="19" t="n">
-        <v>13</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G8" s="19" t="n">
+      <c r="G8" s="20" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G9" s="19" t="n">
+      <c r="G9" s="20" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G10" s="19" t="n">
+      <c r="G10" s="20" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G11" s="19" t="n">
+      <c r="G11" s="20" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">SUM(C3:C16)</f>
@@ -2923,7 +2741,11 @@
       </c>
       <c r="K17" s="0" t="n">
         <f aca="false">SUM(K3:K16)</f>
-        <v>47</v>
+        <v>26</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <f aca="false">SUM(M3:M5)</f>
+        <v>21</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2933,8 +2755,14 @@
       <c r="K19" s="1"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>10</v>
+      </c>
       <c r="D20" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1</v>
@@ -2942,39 +2770,51 @@
       <c r="F20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="0" t="s">
-        <v>89</v>
+      <c r="G20" s="20" t="n">
+        <v>2</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="I20" s="19" t="s">
-        <v>90</v>
+      <c r="I20" s="20" t="s">
+        <v>91</v>
       </c>
       <c r="K20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>4</v>
+      </c>
       <c r="D21" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
+      </c>
+      <c r="G21" s="20" t="n">
+        <v>1</v>
       </c>
       <c r="H21" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I21" s="19" t="s">
-        <v>93</v>
+      <c r="I21" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="K21" s="1"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B22" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="D22" s="2" t="s">
         <v>21</v>
       </c>
@@ -2984,18 +2824,24 @@
       <c r="F22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="0" t="s">
-        <v>94</v>
+      <c r="G22" s="20" t="n">
+        <v>3</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="I22" s="19" t="s">
-        <v>94</v>
+        <v>88</v>
+      </c>
+      <c r="I22" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="K22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="D23" s="10" t="s">
         <v>58</v>
       </c>
@@ -3005,18 +2851,24 @@
       <c r="F23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="0" t="s">
-        <v>94</v>
+      <c r="G23" s="20" t="n">
+        <v>3</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I23" s="19" t="s">
-        <v>95</v>
+      <c r="I23" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="K23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>3</v>
+      </c>
       <c r="D24" s="10" t="s">
         <v>44</v>
       </c>
@@ -3026,14 +2878,14 @@
       <c r="F24" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="0" t="s">
-        <v>90</v>
+      <c r="G24" s="20" t="n">
+        <v>3</v>
       </c>
       <c r="H24" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="I24" s="19" t="s">
-        <v>93</v>
+      <c r="I24" s="20" t="s">
+        <v>94</v>
       </c>
       <c r="K24" s="1"/>
     </row>
@@ -3047,14 +2899,14 @@
       <c r="F25" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="0" t="s">
-        <v>90</v>
+      <c r="G25" s="20" t="n">
+        <v>1</v>
       </c>
       <c r="H25" s="12" t="s">
         <v>62</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K25" s="1"/>
     </row>
@@ -3068,14 +2920,14 @@
       <c r="F26" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="0" t="s">
-        <v>96</v>
+      <c r="G26" s="20" t="n">
+        <v>3</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="K26" s="1"/>
     </row>
@@ -3089,8 +2941,8 @@
       <c r="F27" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="0" t="s">
-        <v>96</v>
+      <c r="G27" s="20" t="n">
+        <v>1</v>
       </c>
       <c r="K27" s="1"/>
     </row>
@@ -3098,8 +2950,8 @@
       <c r="F28" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="G28" s="0" t="s">
-        <v>98</v>
+      <c r="G28" s="20" t="n">
+        <v>2</v>
       </c>
       <c r="K28" s="1"/>
     </row>
@@ -3107,8 +2959,8 @@
       <c r="F29" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="G29" s="0" t="s">
-        <v>98</v>
+      <c r="G29" s="20" t="n">
+        <v>2</v>
       </c>
       <c r="K29" s="1"/>
     </row>
@@ -3122,9 +2974,17 @@
       <c r="K32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C33" s="0" t="n">
+        <f aca="false">SUM(C20:C24)</f>
+        <v>23</v>
+      </c>
       <c r="E33" s="0" t="n">
         <f aca="false">SUM(E20:E32)</f>
         <v>29</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <f aca="false">SUM(G20:G29)</f>
+        <v>21</v>
       </c>
       <c r="I33" s="0" t="n">
         <f aca="false">SUM(I20:I26)</f>

</xml_diff>

<commit_message>
Solucion a consultar object
</commit_message>
<xml_diff>
--- a/Storys/Storys/Hoja1 (version 1).xlsx
+++ b/Storys/Storys/Hoja1 (version 1).xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="92">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -275,46 +275,28 @@
     <t xml:space="preserve">Sprint 5 (29/11/18 – 5/12/18)</t>
   </si>
   <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login Ver. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login Ver. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alta Usuario Ver. 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alta Usuario Ver. 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminacion Estudios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estudios Particular (Analista)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Estudios Particular (Encuestador)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estudios Particular (Analista)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login Ver. 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login Ver. 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marisol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alta Usuario Ver. 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alta Usuario Ver. 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminacion Estudios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alfosno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maribel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">emmanuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliseo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">edgar</t>
   </si>
 </sst>
 </file>
@@ -368,7 +350,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,12 +423,6 @@
         <bgColor rgb="FFE2EFD9"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFE2EFD9"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
@@ -489,7 +465,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -570,8 +546,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -594,7 +578,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFFCDFF"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -611,7 +595,7 @@
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFCDFF"/>
+      <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFC5E0B3"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
@@ -2542,7 +2526,7 @@
   <dimension ref="B1:L34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2555,7 +2539,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="28.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="31.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="32.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="32.27"/>
@@ -2585,129 +2569,89 @@
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="20"/>
-      <c r="D3" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="G3" s="21" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="I3" s="21" t="n">
-        <v>5</v>
-      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="20"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="22"/>
       <c r="J3" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="K3" s="21" t="n">
+      <c r="K3" s="22" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="20"/>
-      <c r="D4" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G4" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="21" t="n">
-        <v>2</v>
-      </c>
+      <c r="C4" s="21"/>
+      <c r="D4" s="20"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="K4" s="21" t="n">
+      <c r="K4" s="22" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="20"/>
-      <c r="G5" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="I5" s="21" t="n">
-        <v>5</v>
-      </c>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="23"/>
       <c r="J5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="21" t="n">
+      <c r="K5" s="22" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="20"/>
-      <c r="G6" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="21" t="n">
-        <v>8</v>
-      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="23"/>
       <c r="J6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K6" s="21" t="n">
+      <c r="K6" s="22" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="20"/>
-      <c r="G7" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="I7" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="23"/>
       <c r="J7" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="K7" s="21" t="n">
+      <c r="K7" s="22" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G8" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="G8" s="22"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G9" s="21" t="n">
-        <v>3</v>
-      </c>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G10" s="21" t="n">
-        <v>1</v>
-      </c>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G11" s="21" t="n">
-        <v>2</v>
-      </c>
+      <c r="G11" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="0" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">SUM(C3:C16)</f>
@@ -2715,15 +2659,15 @@
       </c>
       <c r="E17" s="0" t="n">
         <f aca="false">SUM(E3:E16)</f>
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G17" s="0" t="n">
         <f aca="false">SUM(G3:G16)</f>
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="I17" s="0" t="n">
         <f aca="false">SUM(I3:I16)</f>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="K17" s="0" t="n">
         <f aca="false">SUM(K3:K16)</f>
@@ -2738,13 +2682,13 @@
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E20" s="0" t="n">
         <v>1</v>
@@ -2752,41 +2696,43 @@
       <c r="F20" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="21" t="n">
+      <c r="G20" s="22" t="n">
         <v>2</v>
       </c>
-      <c r="H20" s="12" t="s">
+      <c r="H20" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="22"/>
+      <c r="J20" s="12" t="s">
         <v>66</v>
-      </c>
-      <c r="I20" s="21" t="s">
-        <v>89</v>
       </c>
       <c r="K20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E21" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="21" t="n">
+        <v>89</v>
+      </c>
+      <c r="G21" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="H21" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I21" s="21" t="s">
-        <v>93</v>
+      <c r="H21" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I21" s="22"/>
+      <c r="J21" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="K21" s="1"/>
     </row>
@@ -2806,15 +2752,13 @@
       <c r="F22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="21" t="n">
+      <c r="G22" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="H22" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>94</v>
-      </c>
+      <c r="H22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="22"/>
       <c r="K22" s="1"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2833,15 +2777,13 @@
       <c r="F23" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G23" s="21" t="n">
+      <c r="G23" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" s="21" t="s">
-        <v>95</v>
-      </c>
+      <c r="H23" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="22"/>
       <c r="K23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2860,15 +2802,13 @@
       <c r="F24" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="21" t="n">
+      <c r="G24" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="H24" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="I24" s="21" t="s">
-        <v>93</v>
-      </c>
+      <c r="H24" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="I24" s="22"/>
       <c r="K24" s="1"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2881,14 +2821,11 @@
       <c r="F25" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="G25" s="21" t="n">
+      <c r="G25" s="22" t="n">
         <v>1</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="K25" s="1"/>
     </row>
@@ -2902,14 +2839,11 @@
       <c r="F26" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="21" t="n">
+      <c r="G26" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="H26" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>97</v>
+      <c r="H26" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="K26" s="1"/>
     </row>
@@ -2923,24 +2857,14 @@
       <c r="F27" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G27" s="21" t="n">
+      <c r="G27" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="H27" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="I27" s="21" t="n">
-        <v>2</v>
-      </c>
+      <c r="I27" s="22"/>
       <c r="K27" s="1"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H28" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="I28" s="21" t="n">
-        <v>2</v>
-      </c>
+      <c r="I28" s="22"/>
       <c r="K28" s="1"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2971,7 +2895,7 @@
       <c r="I33" s="0" t="n">
         <v>32</v>
       </c>
-      <c r="J33" s="22"/>
+      <c r="J33" s="24"/>
       <c r="K33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>